<commit_message>
tester for final approach
</commit_message>
<xml_diff>
--- a/real_data/resnet101.xlsx
+++ b/real_data/resnet101.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joanatirana/Desktop/delft-visiting/optimize code/scheduling-jobs/real_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDBBB9B5-911F-EC4B-A9D0-E0A00A3F2B79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83043816-0854-3342-A28D-E8BE9CE4C182}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="16440" activeTab="3" xr2:uid="{7935258D-7BA1-BE4D-B533-9C0418764F7B}"/>
   </bookViews>
@@ -1248,7 +1248,7 @@
   <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1670,7 +1670,7 @@
   <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+      <selection activeCell="N35" sqref="N35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2051,7 +2051,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
-        <v>19200</v>
+        <v>1920</v>
       </c>
       <c r="B35" s="1">
         <v>15755</v>
@@ -2062,7 +2062,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="B36" s="1">
         <v>21</v>

</xml_diff>